<commit_message>
Add n15t40 simulation result. Organise the folder: add the "n15" folder in dgp5.
</commit_message>
<xml_diff>
--- a/simuresult/simulation result documents_com.xlsx
+++ b/simuresult/simulation result documents_com.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20395"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Thesis\Oct_CodingSummary\Simulation\simuresult\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2200767\Documents\Simulation\simuresult\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8DE9D4C-1655-46F2-B0A8-8F438C48B4D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="5910" xr2:uid="{8DF7351A-A98F-448E-B47D-D639264B29EC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="5910"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="12">
   <si>
     <t>N_ctrl</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -64,13 +63,21 @@
   </si>
   <si>
     <t>y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DGP7(dgp6)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -427,19 +434,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E01ADCD-2E64-4D09-9B9A-B94A86243AB6}">
-  <dimension ref="B1:H10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="4" max="6" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="11.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -461,8 +468,11 @@
       <c r="H1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B2">
         <v>10</v>
       </c>
@@ -485,7 +495,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B3">
         <v>10</v>
       </c>
@@ -508,7 +518,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B4">
         <v>10</v>
       </c>
@@ -527,8 +537,11 @@
       <c r="G4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B5">
         <v>15</v>
       </c>
@@ -547,8 +560,11 @@
       <c r="G5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B6">
         <v>15</v>
       </c>
@@ -567,8 +583,11 @@
       <c r="G6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B7">
         <v>15</v>
       </c>
@@ -587,8 +606,11 @@
       <c r="G7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B8">
         <v>20</v>
       </c>
@@ -596,7 +618,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B9">
         <v>20</v>
       </c>
@@ -604,7 +626,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B10">
         <v>20</v>
       </c>
@@ -615,5 +637,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>